<commit_message>
Update VII - PASSED OUT bashir.xlsx
</commit_message>
<xml_diff>
--- a/VII - PASSED OUT bashir.xlsx
+++ b/VII - PASSED OUT bashir.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="1350">
   <si>
     <t>REGISTRATION NUMBER</t>
   </si>
@@ -4069,6 +4069,9 @@
   </si>
   <si>
     <t>03299988852</t>
+  </si>
+  <si>
+    <t>huihuihjkhkjhnjk</t>
   </si>
 </sst>
 </file>
@@ -4464,7 +4467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4473,10 +4476,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G599"/>
+  <dimension ref="A1:G602"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G501" sqref="G501"/>
+      <selection activeCell="D605" sqref="D605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15035,6 +15038,11 @@
     <row r="599" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E599" s="6"/>
     </row>
+    <row r="602" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D602" s="2" t="s">
+        <v>1349</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G597">
     <filterColumn colId="0">

</xml_diff>